<commit_message>
updates for v0.8.0: don't need `/` anymore
</commit_message>
<xml_diff>
--- a/bonds/bonds.xlsx
+++ b/bonds/bonds.xlsx
@@ -283,22 +283,22 @@
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
+          <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
-          <a:prstDash val="solid"/>
         </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
+          <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
-          <a:prstDash val="solid"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
+          <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
-          <a:prstDash val="solid"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -367,6 +367,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1000"/>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="11" width="8.38" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s" s="2">

</xml_diff>